<commit_message>
fix: fix lambda3 not being dynamic
</commit_message>
<xml_diff>
--- a/Типовик 6 - Собственные значения и вектора.xlsx
+++ b/Типовик 6 - Собственные значения и вектора.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Boris\Documents\MIREA\Course2\Vychmat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F49FFC50-9EBF-456A-B4B0-810191FE3B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C21F28-8500-4DE2-9011-98E174693F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5430" yWindow="0" windowWidth="23490" windowHeight="15480" xr2:uid="{230C48AD-2663-48CD-B354-288650DF21D9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{230C48AD-2663-48CD-B354-288650DF21D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -897,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C39C05-0506-4240-8892-3FBD3A4302FB}">
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,74 +933,74 @@
         <v>23</v>
       </c>
       <c r="B2" s="25">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2" s="25">
-        <v>-3</v>
+        <v>-6</v>
       </c>
       <c r="D2" s="25">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F2" s="10">
         <v>0</v>
       </c>
       <c r="H2" s="10">
         <f t="array" ref="H2:H4">MMULT(B2:D4,F2:F4)</f>
-        <v>-3</v>
+        <v>-6</v>
       </c>
       <c r="J2" s="10">
         <f t="array" ref="J2:J4">MMULT(B2:D4,H2:H4)</f>
-        <v>-15</v>
+        <v>-24</v>
       </c>
       <c r="L2" s="10" cm="1">
         <f t="array" ref="L2:L4">MMULT(B2:D4,J2:J4)</f>
-        <v>-63</v>
+        <v>-222</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="25">
+        <v>-1</v>
+      </c>
+      <c r="D3" s="25">
         <v>2</v>
-      </c>
-      <c r="D3" s="25">
-        <v>1</v>
       </c>
       <c r="F3" s="10">
         <v>1</v>
       </c>
       <c r="H3" s="10">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="J3" s="10">
-        <v>2</v>
+        <v>-7</v>
       </c>
       <c r="L3" s="10">
-        <v>-10</v>
+        <v>-73</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="25">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="F4" s="10">
         <v>0</v>
       </c>
       <c r="H4" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J4" s="10">
-        <v>1</v>
+        <v>-16</v>
       </c>
       <c r="L4" s="10">
-        <v>-11</v>
+        <v>-46</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1011,11 +1011,11 @@
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" s="14">
         <f t="array" ref="B8:B10">J2:J4</f>
-        <v>-15</v>
+        <v>-24</v>
       </c>
       <c r="C8" s="17">
         <f t="array" ref="C8:C10">H2:H4</f>
-        <v>-3</v>
+        <v>-6</v>
       </c>
       <c r="D8" s="19">
         <f t="array" ref="D8:D10">F2:F4</f>
@@ -1023,35 +1023,35 @@
       </c>
       <c r="E8" s="12">
         <f t="array" ref="E8:E10">-L2:L4</f>
-        <v>63</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" s="15">
-        <v>2</v>
+        <v>-7</v>
       </c>
       <c r="C9" s="10">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D9" s="20">
         <v>1</v>
       </c>
       <c r="E9" s="13">
-        <v>10</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="16">
-        <v>1</v>
+        <v>-16</v>
       </c>
       <c r="C10" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="21">
         <v>0</v>
       </c>
       <c r="E10" s="9">
-        <v>11</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1060,20 +1060,20 @@
       </c>
       <c r="B13" s="23">
         <f t="array" ref="B13:D15">MINVERSE(B8:D10)</f>
-        <v>-8.3333333333333329E-2</v>
+        <v>-1.388888888888889E-2</v>
       </c>
       <c r="C13" s="23">
         <v>0</v>
       </c>
       <c r="D13" s="23">
-        <v>-0.25</v>
+        <v>-4.1666666666666664E-2</v>
       </c>
       <c r="G13" t="s">
         <v>10</v>
       </c>
       <c r="H13" s="10" cm="1">
         <f t="array" ref="H13:H15">MMULT(B13:D15,E8:E10)</f>
-        <v>-8</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1081,19 +1081,19 @@
         <v>8</v>
       </c>
       <c r="B14" s="23">
-        <v>8.3333333333333329E-2</v>
+        <v>-0.1111111111111111</v>
       </c>
       <c r="C14" s="23">
         <v>0</v>
       </c>
       <c r="D14" s="23">
-        <v>1.25</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="G14" t="s">
         <v>11</v>
       </c>
       <c r="H14" s="10">
-        <v>19</v>
+        <v>-17</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1101,19 +1101,19 @@
         <v>9</v>
       </c>
       <c r="B15" s="23">
-        <v>0</v>
+        <v>-0.20833333333333337</v>
       </c>
       <c r="C15" s="23">
         <v>1</v>
       </c>
       <c r="D15" s="23">
-        <v>-2</v>
+        <v>-0.125</v>
       </c>
       <c r="G15" t="s">
         <v>12</v>
       </c>
       <c r="H15" s="10">
-        <v>-12</v>
+        <v>20.999999999999993</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
@@ -1147,7 +1147,7 @@
         <v>14</v>
       </c>
       <c r="C20" s="5">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -1161,7 +1161,7 @@
         <v>15</v>
       </c>
       <c r="C21" s="22">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="22"/>
@@ -1214,12 +1214,12 @@
       <c r="F25" s="5"/>
       <c r="G25" s="5">
         <f>C23*E25+$H$13*E25</f>
-        <v>-7</v>
+        <v>-4</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="5">
         <f>C23*G25+$H$14*E25</f>
-        <v>12</v>
+        <v>-21</v>
       </c>
       <c r="J25" s="6"/>
     </row>
@@ -1250,7 +1250,7 @@
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="4">
         <f t="array" ref="B28:B30">E25*$J$2:$J$4+G25*$H$2:$H$4+I25*$F$2:$F$4</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -1263,7 +1263,7 @@
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="4">
-        <v>0</v>
+        <v>-24</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -1276,7 +1276,7 @@
     </row>
     <row r="30" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="7">
-        <v>-6</v>
+        <v>-24</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -1294,7 +1294,7 @@
       </c>
       <c r="C32" s="34">
         <f>C20</f>
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -1331,12 +1331,12 @@
       <c r="F34" s="5"/>
       <c r="G34" s="5">
         <f>C32*E34+$H$13*E34</f>
-        <v>-5</v>
+        <v>-8</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="5">
         <f>C32*G34+$H$14*E34</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J34" s="6"/>
     </row>
@@ -1367,7 +1367,7 @@
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="4">
         <f t="array" ref="B37:B39">E34*$J$2:$J$4+G34*$H$2:$H$4+I34*$F$2:$F$4</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -1380,7 +1380,7 @@
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="4">
-        <v>-4</v>
+        <v>8</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -1393,7 +1393,7 @@
     </row>
     <row r="39" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="7">
-        <v>-4</v>
+        <v>-32</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
@@ -1410,7 +1410,8 @@
         <v>16</v>
       </c>
       <c r="C41" s="34">
-        <v>4</v>
+        <f>C21</f>
+        <v>7</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -1447,12 +1448,12 @@
       <c r="F43" s="5"/>
       <c r="G43" s="5">
         <f>C41*E43+$H$13*E43</f>
-        <v>-4</v>
+        <v>2</v>
       </c>
       <c r="H43" s="5"/>
       <c r="I43" s="5">
         <f>C41*G43+$H$14*E43</f>
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="J43" s="6"/>
     </row>
@@ -1483,7 +1484,7 @@
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="4">
         <f t="array" ref="B46:B48">E43*$J$2:$J$4+G43*$H$2:$H$4+I43*$F$2:$F$4</f>
-        <v>-3</v>
+        <v>-36</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
@@ -1496,7 +1497,7 @@
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" s="4">
-        <v>-3</v>
+        <v>-12</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
@@ -1509,7 +1510,7 @@
     </row>
     <row r="48" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="7">
-        <v>-3</v>
+        <v>-12</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
@@ -1531,7 +1532,7 @@
       <c r="F51" s="2"/>
       <c r="G51" s="35">
         <f t="array" ref="G51:G53">B28:B30</f>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.25">
@@ -1548,7 +1549,7 @@
         <v>20</v>
       </c>
       <c r="G52" s="36">
-        <v>0</v>
+        <v>-24</v>
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
@@ -1558,7 +1559,7 @@
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
       <c r="G53" s="36">
-        <v>-6</v>
+        <v>-24</v>
       </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.25">
@@ -1577,7 +1578,7 @@
       <c r="F55" s="5"/>
       <c r="G55" s="36">
         <f t="array" ref="G55:G57">B37:B39</f>
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.25">
@@ -1587,14 +1588,14 @@
       </c>
       <c r="D56" s="5">
         <f>C32</f>
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="E56" s="5"/>
       <c r="F56" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G56" s="36">
-        <v>-4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.25">
@@ -1604,7 +1605,7 @@
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
       <c r="G57" s="36">
-        <v>-4</v>
+        <v>-32</v>
       </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.25">
@@ -1623,7 +1624,7 @@
       <c r="F59" s="5"/>
       <c r="G59" s="36">
         <f t="array" ref="G59:G61">B46:B48</f>
-        <v>-3</v>
+        <v>-36</v>
       </c>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.25">
@@ -1633,14 +1634,14 @@
       </c>
       <c r="D60" s="5">
         <f>C41</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E60" s="5"/>
       <c r="F60" s="5" t="s">
         <v>22</v>
       </c>
       <c r="G60" s="36">
-        <v>-3</v>
+        <v>-12</v>
       </c>
     </row>
     <row r="61" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1650,7 +1651,7 @@
       <c r="E61" s="8"/>
       <c r="F61" s="8"/>
       <c r="G61" s="37">
-        <v>-3</v>
+        <v>-12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>